<commit_message>
Updates for Framework and CVC Project up to 6/19/2018
</commit_message>
<xml_diff>
--- a/doc/messagesDefinition-v1.xlsx
+++ b/doc/messagesDefinition-v1.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_wk\_p\dds-launchpad-iiot-poc-psg-pub\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_wk\_p\dds-launchpad-iiot-cvc-cloud-dev\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{151F9272-230D-463C-9898-2E46BEF61504}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D30805-0A35-4F1C-9920-E78EA61A1936}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21317" windowHeight="12394" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21317" windowHeight="12394" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="messageSchema" sheetId="1" r:id="rId1"/>
-    <sheet name="sample01" sheetId="2" r:id="rId2"/>
-    <sheet name="sample02" sheetId="3" r:id="rId3"/>
+    <sheet name="sample01" sheetId="4" r:id="rId2"/>
+    <sheet name="sampleold" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="59">
   <si>
     <t>timestamp</t>
   </si>
@@ -110,24 +110,6 @@
     <t>accoustic</t>
   </si>
   <si>
-    <t>[200,130,110,111,112,113,114,115,116,117]</t>
-  </si>
-  <si>
-    <t>[110,240,205,206,207,208,209,210,211,212]</t>
-  </si>
-  <si>
-    <t>[300,140,100,300,301,302,303,304,305,306]</t>
-  </si>
-  <si>
-    <t>[100,200,220,225,226,227,228,229,230,231]</t>
-  </si>
-  <si>
-    <t>[301,130,104,345,234,235,236,237,238,239]</t>
-  </si>
-  <si>
-    <t>[110,203,228,215,200,201,202,203,204,205]</t>
-  </si>
-  <si>
     <t>[110,240,205,206,207,208,209,210,211,212,110,240,205,206,217,208,219,210,211,212,110,240,205,206,207,208,209,210,211,212,110,240,205,206,207,208,209,210,211,212,110,240,205,206,207,208,209,210,211,212,110,240,205,206,207,208,209,110,211,212,110,240,111,194,132,222,223,216,211,212,110,241,115,226,227,208,209,210,211,212,110,240,205,126,207,201,109,210,211,112,113,241,105,206,107,201,219,122,211,112]</t>
   </si>
   <si>
@@ -192,6 +174,36 @@
   </si>
   <si>
     <t>tempInternal</t>
+  </si>
+  <si>
+    <t>sourceName</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>activity</t>
+  </si>
+  <si>
+    <t>cvcdev</t>
+  </si>
+  <si>
+    <t>locdevsrc</t>
+  </si>
+  <si>
+    <t>Prime Gas</t>
+  </si>
+  <si>
+    <t>activityFlag</t>
+  </si>
+  <si>
+    <t>eventType</t>
+  </si>
+  <si>
+    <t>geolocation</t>
   </si>
 </sst>
 </file>
@@ -553,7 +565,10 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -584,28 +599,19 @@
         <v>8</v>
       </c>
       <c r="E1" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="F1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" t="s">
         <v>52</v>
-      </c>
-      <c r="G1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H1" t="s">
-        <v>54</v>
-      </c>
-      <c r="I1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.4">
@@ -628,22 +634,13 @@
         <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="I2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.4">
@@ -659,6 +656,9 @@
       <c r="D3" t="s">
         <v>16</v>
       </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
@@ -667,24 +667,6 @@
       <c r="F4">
         <v>0</v>
       </c>
-      <c r="G4">
-        <v>-255</v>
-      </c>
-      <c r="H4">
-        <v>-255</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
@@ -693,63 +675,15 @@
       <c r="F5">
         <v>7</v>
       </c>
-      <c r="G5">
-        <v>4096</v>
-      </c>
-      <c r="H5">
-        <v>4096</v>
-      </c>
-      <c r="I5">
-        <v>4096</v>
-      </c>
-      <c r="J5">
-        <v>1000</v>
-      </c>
-      <c r="K5">
-        <v>255</v>
-      </c>
-      <c r="L5">
-        <v>10000</v>
-      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="G6">
-        <v>-50</v>
-      </c>
-      <c r="H6">
-        <v>-50</v>
-      </c>
-      <c r="I6">
-        <v>2700</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>5</v>
-      </c>
-      <c r="G7">
-        <v>200</v>
-      </c>
-      <c r="H7">
-        <v>200</v>
-      </c>
-      <c r="I7">
-        <v>3600</v>
-      </c>
-      <c r="K7">
-        <v>255</v>
-      </c>
-      <c r="L7">
-        <v>10000</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.4">
@@ -785,6 +719,148 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BC643C2-C396-441B-97F6-B10430F228C5}">
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="24.3046875" customWidth="1"/>
+    <col min="2" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="14.3046875" customWidth="1"/>
+    <col min="5" max="5" width="20.15234375" customWidth="1"/>
+    <col min="6" max="6" width="13.53515625" customWidth="1"/>
+    <col min="7" max="8" width="12.53515625" customWidth="1"/>
+    <col min="9" max="9" width="19.23046875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" t="s">
+        <v>55</v>
+      </c>
+      <c r="G8">
+        <v>77.345100000000002</v>
+      </c>
+      <c r="H8">
+        <v>80.345600000000005</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L17"/>
   <sheetViews>
@@ -823,13 +899,13 @@
         <v>24</v>
       </c>
       <c r="F1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="H1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="I1" t="s">
         <v>3</v>
@@ -993,7 +1069,7 @@
         <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
         <v>19</v>
@@ -1017,10 +1093,10 @@
         <v>100</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.4">
@@ -1028,7 +1104,7 @@
         <v>10000</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D9" t="s">
         <v>22</v>
@@ -1052,10 +1128,10 @@
         <v>100</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.4">
@@ -1063,7 +1139,7 @@
         <v>20000</v>
       </c>
       <c r="C10" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D10" t="s">
         <v>23</v>
@@ -1087,10 +1163,10 @@
         <v>100</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.4">
@@ -1098,7 +1174,7 @@
         <v>5000</v>
       </c>
       <c r="C11" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D11" t="s">
         <v>19</v>
@@ -1122,10 +1198,10 @@
         <v>100</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.4">
@@ -1133,7 +1209,7 @@
         <v>10000</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D12" t="s">
         <v>22</v>
@@ -1157,10 +1233,10 @@
         <v>100</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.4">
@@ -1168,7 +1244,7 @@
         <v>20000</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D13" t="s">
         <v>23</v>
@@ -1192,10 +1268,10 @@
         <v>100</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.4">
@@ -1203,7 +1279,7 @@
         <v>15000</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D14" t="s">
         <v>19</v>
@@ -1227,10 +1303,10 @@
         <v>100</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.4">
@@ -1238,7 +1314,7 @@
         <v>10000</v>
       </c>
       <c r="C15" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D15" t="s">
         <v>22</v>
@@ -1262,10 +1338,10 @@
         <v>100</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.4">
@@ -1273,7 +1349,7 @@
         <v>20000</v>
       </c>
       <c r="C16" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D16" t="s">
         <v>23</v>
@@ -1297,10 +1373,10 @@
         <v>100</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.4">
@@ -1312,202 +1388,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D8977B2-AAE5-4B3C-96B4-E86BDEB69204}">
-  <dimension ref="A1:L11"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="16.07421875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.69140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.84375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.3828125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.4609375" customWidth="1"/>
-    <col min="7" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="11.07421875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.61328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="36.69140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H1" t="s">
-        <v>54</v>
-      </c>
-      <c r="I1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>100</v>
-      </c>
-      <c r="H2">
-        <v>105</v>
-      </c>
-      <c r="I2">
-        <v>3000</v>
-      </c>
-      <c r="J2">
-        <v>10</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A3">
-        <v>10000</v>
-      </c>
-      <c r="C3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3">
-        <v>3</v>
-      </c>
-      <c r="G3">
-        <v>50</v>
-      </c>
-      <c r="H3">
-        <v>60</v>
-      </c>
-      <c r="I3">
-        <v>2500</v>
-      </c>
-      <c r="J3">
-        <v>10</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A4">
-        <v>10000</v>
-      </c>
-      <c r="C4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4">
-        <v>4</v>
-      </c>
-      <c r="G4">
-        <v>-20</v>
-      </c>
-      <c r="H4">
-        <v>-10</v>
-      </c>
-      <c r="I4">
-        <v>3500</v>
-      </c>
-      <c r="J4">
-        <v>10</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="K5" s="2"/>
-      <c r="L5" s="3"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="K6" s="2"/>
-      <c r="L6" s="3"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="K7" s="2"/>
-      <c r="L7" s="3"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="K8" s="2"/>
-      <c r="L8" s="3"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="K9" s="2"/>
-      <c r="L9" s="3"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="K10" s="2"/>
-      <c r="L10" s="3"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>